<commit_message>
Feat(all) : Implemented Excel
</commit_message>
<xml_diff>
--- a/ReportService/BackgroundService/Reports/report_Antalya.xlsx
+++ b/ReportService/BackgroundService/Reports/report_Antalya.xlsx
@@ -5,19 +5,25 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Antalya" sheetId="1" r:id="rId1"/>
+    <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Belirttiğiniz Konumda ki Kişi Sayısı</t>
+    <t>Konum</t>
   </si>
   <si>
-    <t>Belirttiğiniz Konumda ki Gsm Sayısı</t>
+    <t>Kişi Sayısı</t>
+  </si>
+  <si>
+    <t>Telefon Numarası Sayısı</t>
+  </si>
+  <si>
+    <t>Antalya</t>
   </si>
 </sst>
 </file>
@@ -63,14 +69,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.258861541748047" customWidth="1"/>
-    <col min="2" max="2" width="31.232820510864258" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.544389724731445" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -80,12 +87,18 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="0">
+      <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="0">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0">
         <v>2</v>
       </c>
     </row>

</xml_diff>